<commit_message>
run 1st part test again and2nd part test
</commit_message>
<xml_diff>
--- a/yolov5/PerformanceResults.xlsx
+++ b/yolov5/PerformanceResults.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DevProj\dmf_recovery_system\yolov5\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\courses\dmf\dmf_recovery_system\yolov5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B79608C1-7BC3-453E-8C06-18EB25BB0C0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0266A783-17EA-4D8B-9D19-3CF3198FA2AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D0A2016D-912D-447E-92D4-CA5CFE1E8E2E}"/>
+    <workbookView xWindow="1860" yWindow="1860" windowWidth="16800" windowHeight="9710" xr2:uid="{D0A2016D-912D-447E-92D4-CA5CFE1E8E2E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,17 +27,40 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
+  <si>
+    <t>Average</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ave Time of the Detection Part (pre + detect + post)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Average Time of the YOLOv5 Detection (only detect)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t># droplet</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Run Time (ms)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -76,13 +99,19 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -414,79 +443,261 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51935BBD-CEDF-4E29-B151-8F139D9BD44F}">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:N8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:J1"/>
+      <selection activeCell="O17" sqref="O17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14"/>
+  <cols>
+    <col min="1" max="1" width="12.58203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1">
+    <row r="1" spans="1:14">
+      <c r="B1">
+        <v>0</v>
+      </c>
+      <c r="C1">
         <v>1</v>
       </c>
-      <c r="B1">
+      <c r="D1">
         <v>2</v>
       </c>
-      <c r="C1">
+      <c r="E1">
         <v>3</v>
       </c>
-      <c r="D1">
+      <c r="F1">
         <v>4</v>
       </c>
-      <c r="E1">
+      <c r="G1">
         <v>5</v>
       </c>
-      <c r="F1">
+      <c r="H1">
         <v>6</v>
       </c>
-      <c r="G1">
+      <c r="I1">
         <v>7</v>
       </c>
-      <c r="H1">
+      <c r="J1">
         <v>8</v>
       </c>
-      <c r="I1">
+      <c r="K1">
         <v>9</v>
       </c>
-      <c r="J1">
+      <c r="L1">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2">
+    <row r="2" spans="1:14">
+      <c r="C2">
         <v>478.90908669999999</v>
       </c>
-      <c r="B2">
+      <c r="D2">
         <v>471.32913680000001</v>
       </c>
-      <c r="C2">
+      <c r="E2">
         <v>471.03545830000002</v>
       </c>
-      <c r="D2">
+      <c r="F2">
         <v>464.28478890000002</v>
       </c>
-      <c r="E2">
+      <c r="G2">
         <v>464.79787040000002</v>
       </c>
-      <c r="F2">
+      <c r="H2">
         <v>477.87166960000002</v>
       </c>
-      <c r="G2">
+      <c r="I2">
         <v>458.87647709999999</v>
       </c>
-      <c r="H2">
+      <c r="J2">
         <v>471.02305330000002</v>
       </c>
-      <c r="I2">
+      <c r="K2">
         <v>469.15308670000002</v>
       </c>
-      <c r="J2">
+      <c r="L2">
         <v>474.7280667</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1">
+        <v>0</v>
+      </c>
+      <c r="C4" s="1">
+        <v>1</v>
+      </c>
+      <c r="D4" s="1">
+        <v>2</v>
+      </c>
+      <c r="E4" s="1">
+        <v>3</v>
+      </c>
+      <c r="F4" s="1">
+        <v>4</v>
+      </c>
+      <c r="G4" s="1">
+        <v>5</v>
+      </c>
+      <c r="H4" s="1">
+        <v>6</v>
+      </c>
+      <c r="I4" s="1">
+        <v>7</v>
+      </c>
+      <c r="J4" s="1">
+        <v>8</v>
+      </c>
+      <c r="K4" s="1">
+        <v>9</v>
+      </c>
+      <c r="L4" s="1">
+        <v>10</v>
+      </c>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
+      <c r="A5" s="1"/>
+      <c r="B5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+    </row>
+    <row r="6" spans="1:14">
+      <c r="A6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="1">
+        <v>353.70377999999988</v>
+      </c>
+      <c r="C6" s="1">
+        <v>357.05817333333317</v>
+      </c>
+      <c r="D6" s="1">
+        <v>343.73861999999986</v>
+      </c>
+      <c r="E6" s="1">
+        <v>344.2699933333331</v>
+      </c>
+      <c r="F6" s="1">
+        <v>347.89613999999972</v>
+      </c>
+      <c r="G6" s="1">
+        <v>351.1491666666663</v>
+      </c>
+      <c r="H6" s="1">
+        <v>355.95284666666663</v>
+      </c>
+      <c r="I6" s="1">
+        <v>344.48259333333311</v>
+      </c>
+      <c r="J6" s="1">
+        <v>339.54561333333305</v>
+      </c>
+      <c r="K6" s="1">
+        <v>344.88387333333333</v>
+      </c>
+      <c r="L6" s="1">
+        <v>348.26161999999977</v>
+      </c>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1">
+        <f>AVERAGE(B6:L6)</f>
+        <v>348.2674927272725</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14">
+      <c r="A7" s="1"/>
+      <c r="B7" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+    </row>
+    <row r="8" spans="1:14">
+      <c r="A8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="1">
+        <f>1.6+67.5+1</f>
+        <v>70.099999999999994</v>
+      </c>
+      <c r="C8" s="1">
+        <f>0.9+67.7+0.7</f>
+        <v>69.300000000000011</v>
+      </c>
+      <c r="D8" s="1">
+        <f>0.9+67.4+0.8</f>
+        <v>69.100000000000009</v>
+      </c>
+      <c r="E8" s="1">
+        <f>1+66.6+1.1</f>
+        <v>68.699999999999989</v>
+      </c>
+      <c r="F8" s="1">
+        <f>0.6+68.4+0.8</f>
+        <v>69.8</v>
+      </c>
+      <c r="G8" s="1">
+        <f>0.7+69.4+0.5</f>
+        <v>70.600000000000009</v>
+      </c>
+      <c r="H8" s="1">
+        <f>0.9+69.8+0.5</f>
+        <v>71.2</v>
+      </c>
+      <c r="I8" s="1">
+        <f>0.7+66+0.8</f>
+        <v>67.5</v>
+      </c>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1">
+        <f>1+69.1+0.7</f>
+        <v>70.8</v>
+      </c>
+      <c r="L8" s="1">
+        <f>0.7+70+0.9</f>
+        <v>71.600000000000009</v>
+      </c>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1">
+        <f>(SUM(B8:I8) + SUM(K8:L8)) / 10</f>
+        <v>69.86999999999999</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B5:N5"/>
+    <mergeCell ref="B7:N7"/>
+  </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>